<commit_message>
Moved engineering cal parameters to notes
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE02SHSP_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_CE02SHSP_00001.xlsx
@@ -2487,11 +2487,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
+      <selection pane="bottomLeft" activeCell="I50" sqref="I50:P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="I48" s="16"/>
     </row>
-    <row r="49" spans="1:9" s="13" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="13" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A49" s="29"/>
       <c r="B49" s="29"/>
       <c r="C49" s="29"/>
@@ -3739,33 +3739,32 @@
       <c r="H49" s="30"/>
       <c r="I49" s="29"/>
     </row>
-    <row r="50" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
+    <row r="50" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="B50" t="s">
+      <c r="J50" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="K50" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D50" s="20">
+      <c r="L50" s="20">
         <v>1</v>
       </c>
-      <c r="E50" t="s">
+      <c r="M50" t="s">
         <v>97</v>
       </c>
-      <c r="F50" s="35" t="s">
+      <c r="N50" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="G50" s="16"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="16"/>
-    </row>
-    <row r="51" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="O50" s="16"/>
+      <c r="P50" s="32"/>
+    </row>
+    <row r="51" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:E54"/>
   <phoneticPr fontId="32" type="noConversion"/>

</xml_diff>